<commit_message>
Added use_lims argument and Aquathermie plots
</commit_message>
<xml_diff>
--- a/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
+++ b/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
@@ -521,7 +521,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47522672453</v>
+        <v>45096.49076744096</v>
       </c>
     </row>
     <row r="3">
@@ -538,7 +538,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47522672453</v>
+        <v>45096.49076744096</v>
       </c>
     </row>
     <row r="4">
@@ -555,7 +555,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47522672453</v>
+        <v>45096.49076744096</v>
       </c>
     </row>
     <row r="5">
@@ -572,7 +572,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47522672453</v>
+        <v>45096.49076744096</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +630,7 @@
         <v>-0.00035</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47373502315</v>
+        <v>45096.48926726852</v>
       </c>
     </row>
     <row r="3">
@@ -647,7 +647,7 @@
         <v>-0.00035</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47373502315</v>
+        <v>45096.48926726852</v>
       </c>
     </row>
     <row r="4">
@@ -664,7 +664,7 @@
         <v>-0.00035</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47373502315</v>
+        <v>45096.48926726852</v>
       </c>
     </row>
     <row r="5">
@@ -681,7 +681,7 @@
         <v>-0.00035</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47373502315</v>
+        <v>45096.48926726852</v>
       </c>
     </row>
     <row r="6">
@@ -698,7 +698,7 @@
         <v>-0.00035</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45063.47373502315</v>
+        <v>45096.48926726852</v>
       </c>
     </row>
     <row r="7">
@@ -715,7 +715,7 @@
         <v>-0.00035</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45063.47373502315</v>
+        <v>45096.48926726852</v>
       </c>
     </row>
     <row r="8">
@@ -732,7 +732,7 @@
         <v>-0.00035</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>45063.47373502315</v>
+        <v>45096.48926726852</v>
       </c>
     </row>
   </sheetData>
@@ -790,7 +790,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47393028935</v>
+        <v>45096.48950741898</v>
       </c>
     </row>
     <row r="3">
@@ -807,7 +807,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47393028935</v>
+        <v>45096.48950741898</v>
       </c>
     </row>
     <row r="4">
@@ -824,7 +824,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47393028935</v>
+        <v>45096.48950741898</v>
       </c>
     </row>
     <row r="5">
@@ -841,7 +841,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.4739305787</v>
+        <v>45096.4895075926</v>
       </c>
     </row>
     <row r="6">
@@ -858,7 +858,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45063.47393028935</v>
+        <v>45096.48950741898</v>
       </c>
     </row>
   </sheetData>
@@ -916,7 +916,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.4741622338</v>
+        <v>45096.48980850694</v>
       </c>
     </row>
     <row r="3">
@@ -933,7 +933,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.4741622338</v>
+        <v>45096.48980850694</v>
       </c>
     </row>
     <row r="4">
@@ -950,7 +950,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.4741622338</v>
+        <v>45096.48980850694</v>
       </c>
     </row>
     <row r="5">
@@ -967,7 +967,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47416253472</v>
+        <v>45096.48980870371</v>
       </c>
     </row>
   </sheetData>
@@ -1025,7 +1025,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47427172454</v>
+        <v>45096.48990774305</v>
       </c>
     </row>
     <row r="3">
@@ -1042,7 +1042,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47427172454</v>
+        <v>45096.48990774305</v>
       </c>
     </row>
     <row r="4">
@@ -1059,7 +1059,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47427172454</v>
+        <v>45096.48990774305</v>
       </c>
     </row>
     <row r="5">
@@ -1076,7 +1076,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47427172454</v>
+        <v>45096.48990774305</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1134,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47431611111</v>
+        <v>45096.48995410879</v>
       </c>
     </row>
     <row r="3">
@@ -1151,7 +1151,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47431611111</v>
+        <v>45096.48995410879</v>
       </c>
     </row>
     <row r="4">
@@ -1168,7 +1168,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47431611111</v>
+        <v>45096.48995410879</v>
       </c>
     </row>
   </sheetData>
@@ -1226,7 +1226,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.4743762037</v>
+        <v>45096.49000885417</v>
       </c>
     </row>
     <row r="3">
@@ -1243,7 +1243,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.4743762037</v>
+        <v>45096.49000885417</v>
       </c>
     </row>
     <row r="4">
@@ -1260,7 +1260,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47437631944</v>
+        <v>45096.49000898148</v>
       </c>
     </row>
   </sheetData>
@@ -1318,7 +1318,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47450746527</v>
+        <v>45096.49013689814</v>
       </c>
     </row>
     <row r="3">
@@ -1335,7 +1335,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47450769676</v>
+        <v>45096.49013703704</v>
       </c>
     </row>
     <row r="4">
@@ -1352,7 +1352,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47450769676</v>
+        <v>45096.49013703704</v>
       </c>
     </row>
     <row r="5">
@@ -1369,7 +1369,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47450746527</v>
+        <v>45096.49013689814</v>
       </c>
     </row>
     <row r="6">
@@ -1386,7 +1386,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45063.47450746527</v>
+        <v>45096.49013689814</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1444,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47461957176</v>
+        <v>45096.4902321412</v>
       </c>
     </row>
     <row r="3">
@@ -1461,7 +1461,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47461971065</v>
+        <v>45096.49023223379</v>
       </c>
     </row>
     <row r="4">
@@ -1478,7 +1478,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47461971065</v>
+        <v>45096.49023223379</v>
       </c>
     </row>
     <row r="5">
@@ -1495,7 +1495,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47461957176</v>
+        <v>45096.4902321412</v>
       </c>
     </row>
   </sheetData>
@@ -1553,7 +1553,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.4746488426</v>
+        <v>45096.49025758102</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1611,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47468457176</v>
+        <v>45096.49029898148</v>
       </c>
     </row>
     <row r="3">
@@ -1628,7 +1628,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47468466435</v>
+        <v>45096.49029907407</v>
       </c>
     </row>
     <row r="4">
@@ -1645,7 +1645,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47468457176</v>
+        <v>45096.49029898148</v>
       </c>
     </row>
   </sheetData>
@@ -1703,7 +1703,7 @@
         <v>-2.48e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47243916667</v>
+        <v>45096.48779674769</v>
       </c>
     </row>
     <row r="3">
@@ -1720,7 +1720,7 @@
         <v>-2.48e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47243935186</v>
+        <v>45096.48779690972</v>
       </c>
     </row>
     <row r="4">
@@ -1737,7 +1737,7 @@
         <v>-2.48e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47243916667</v>
+        <v>45096.48779674769</v>
       </c>
     </row>
     <row r="5">
@@ -1754,7 +1754,7 @@
         <v>-2.48e-05</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47243916667</v>
+        <v>45096.48779674769</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1812,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47474447916</v>
+        <v>45096.49035333333</v>
       </c>
     </row>
     <row r="3">
@@ -1829,7 +1829,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47474460648</v>
+        <v>45096.4903534375</v>
       </c>
     </row>
     <row r="4">
@@ -1846,7 +1846,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47474460648</v>
+        <v>45096.4903534375</v>
       </c>
     </row>
   </sheetData>
@@ -1904,7 +1904,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47480798611</v>
+        <v>45096.4904037963</v>
       </c>
     </row>
     <row r="3">
@@ -1921,7 +1921,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47480798611</v>
+        <v>45096.4904037963</v>
       </c>
     </row>
     <row r="4">
@@ -1938,7 +1938,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47480798611</v>
+        <v>45096.4904037963</v>
       </c>
     </row>
     <row r="5">
@@ -1955,7 +1955,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47480798611</v>
+        <v>45096.4904037963</v>
       </c>
     </row>
   </sheetData>
@@ -2013,7 +2013,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47500119213</v>
+        <v>45096.49057321759</v>
       </c>
     </row>
     <row r="3">
@@ -2030,7 +2030,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47500130787</v>
+        <v>45096.49057332176</v>
       </c>
     </row>
     <row r="4">
@@ -2047,7 +2047,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47500130787</v>
+        <v>45096.49057332176</v>
       </c>
     </row>
     <row r="5">
@@ -2064,7 +2064,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47500130787</v>
+        <v>45096.49057332176</v>
       </c>
     </row>
     <row r="6">
@@ -2081,7 +2081,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45063.47500130787</v>
+        <v>45096.49057332176</v>
       </c>
     </row>
   </sheetData>
@@ -2139,7 +2139,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47502335648</v>
+        <v>45096.49059289352</v>
       </c>
     </row>
     <row r="3">
@@ -2156,7 +2156,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47502335648</v>
+        <v>45096.49059289352</v>
       </c>
     </row>
     <row r="4">
@@ -2173,7 +2173,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47502335648</v>
+        <v>45096.49059289352</v>
       </c>
     </row>
     <row r="5">
@@ -2190,7 +2190,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47502335648</v>
+        <v>45096.49059289352</v>
       </c>
     </row>
   </sheetData>
@@ -2248,7 +2248,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47517956018</v>
+        <v>45096.49073003473</v>
       </c>
     </row>
     <row r="3">
@@ -2265,7 +2265,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47517972222</v>
+        <v>45096.49073011574</v>
       </c>
     </row>
     <row r="4">
@@ -2282,7 +2282,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47517972222</v>
+        <v>45096.49073011574</v>
       </c>
     </row>
     <row r="5">
@@ -2299,7 +2299,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47517956018</v>
+        <v>45096.49073003473</v>
       </c>
     </row>
   </sheetData>
@@ -2357,7 +2357,7 @@
         <v>-1e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47261012731</v>
+        <v>45096.48796245371</v>
       </c>
     </row>
     <row r="3">
@@ -2374,7 +2374,7 @@
         <v>-1e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47261012731</v>
+        <v>45096.48796245371</v>
       </c>
     </row>
     <row r="4">
@@ -2391,7 +2391,7 @@
         <v>-1e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47261012731</v>
+        <v>45096.48796245371</v>
       </c>
     </row>
   </sheetData>
@@ -2449,7 +2449,7 @@
         <v>-6e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47278454861</v>
+        <v>45096.48813849537</v>
       </c>
     </row>
     <row r="3">
@@ -2466,7 +2466,7 @@
         <v>-6e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.4727847338</v>
+        <v>45096.48813861111</v>
       </c>
     </row>
     <row r="4">
@@ -2483,7 +2483,7 @@
         <v>-6e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.4727847338</v>
+        <v>45096.48813861111</v>
       </c>
     </row>
     <row r="5">
@@ -2500,7 +2500,7 @@
         <v>-6e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47278454861</v>
+        <v>45096.48813849537</v>
       </c>
     </row>
   </sheetData>
@@ -2558,7 +2558,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47304047454</v>
+        <v>45096.48839530093</v>
       </c>
     </row>
     <row r="3">
@@ -2575,7 +2575,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47304047454</v>
+        <v>45096.48839530093</v>
       </c>
     </row>
     <row r="4">
@@ -2592,7 +2592,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47304070602</v>
+        <v>45096.48839552084</v>
       </c>
     </row>
     <row r="5">
@@ -2609,7 +2609,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47304070602</v>
+        <v>45096.48839552084</v>
       </c>
     </row>
   </sheetData>
@@ -2667,7 +2667,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47319918982</v>
+        <v>45096.48860040509</v>
       </c>
     </row>
     <row r="3">
@@ -2684,7 +2684,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47319918982</v>
+        <v>45096.48860040509</v>
       </c>
     </row>
     <row r="4">
@@ -2701,7 +2701,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47319934027</v>
+        <v>45096.4886006713</v>
       </c>
     </row>
     <row r="5">
@@ -2718,7 +2718,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47319918982</v>
+        <v>45096.48860040509</v>
       </c>
     </row>
     <row r="6">
@@ -2735,7 +2735,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45063.47319918982</v>
+        <v>45096.48860040509</v>
       </c>
     </row>
   </sheetData>
@@ -2793,7 +2793,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47331384259</v>
+        <v>45096.48873192129</v>
       </c>
     </row>
     <row r="3">
@@ -2810,7 +2810,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47331384259</v>
+        <v>45096.48873192129</v>
       </c>
     </row>
     <row r="4">
@@ -2827,7 +2827,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.47331384259</v>
+        <v>45096.48873192129</v>
       </c>
     </row>
     <row r="5">
@@ -2844,7 +2844,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47331384259</v>
+        <v>45096.48873192129</v>
       </c>
     </row>
   </sheetData>
@@ -2902,7 +2902,7 @@
         <v>-0.0003</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45068.66270355686</v>
+        <v>45096.48891115741</v>
       </c>
     </row>
     <row r="3">
@@ -2919,7 +2919,7 @@
         <v>-0.0003</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45068.66270355686</v>
+        <v>45096.48891115741</v>
       </c>
     </row>
     <row r="4">
@@ -2936,7 +2936,7 @@
         <v>-0.0003</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45068.66270355686</v>
+        <v>45096.48891115741</v>
       </c>
     </row>
     <row r="5">
@@ -2953,7 +2953,7 @@
         <v>-0.0003</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45068.66270355686</v>
+        <v>45096.48891115741</v>
       </c>
     </row>
   </sheetData>
@@ -3011,7 +3011,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45063.47355284722</v>
+        <v>45096.48905635416</v>
       </c>
     </row>
     <row r="3">
@@ -3028,7 +3028,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45063.47355284722</v>
+        <v>45096.48905635416</v>
       </c>
     </row>
     <row r="4">
@@ -3045,7 +3045,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45063.4735530787</v>
+        <v>45096.4890566088</v>
       </c>
     </row>
     <row r="5">
@@ -3062,7 +3062,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45063.47355284722</v>
+        <v>45096.48905635416</v>
       </c>
     </row>
     <row r="6">
@@ -3079,7 +3079,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45063.47355284722</v>
+        <v>45096.48905635416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ICAS: End of year run 2024
</commit_message>
<xml_diff>
--- a/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
+++ b/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
@@ -521,7 +521,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.49076744096</v>
+        <v>45096.49076744213</v>
       </c>
     </row>
     <row r="3">
@@ -538,7 +538,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.49076744096</v>
+        <v>45096.49076744213</v>
       </c>
     </row>
     <row r="4">
@@ -555,7 +555,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.49076744096</v>
+        <v>45096.49076744213</v>
       </c>
     </row>
     <row r="5">
@@ -572,7 +572,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.49076744096</v>
+        <v>45096.49076744213</v>
       </c>
     </row>
   </sheetData>
@@ -624,13 +624,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-6.264577777444832e-67</v>
+        <v>-1.148933078226618e-72</v>
       </c>
       <c r="D2" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48926726852</v>
+        <v>45657.57153850694</v>
       </c>
     </row>
     <row r="3">
@@ -641,13 +641,13 @@
         <v>41682</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.003524281042905766</v>
+        <v>-7.373037232174746e-77</v>
       </c>
       <c r="D3" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48926726852</v>
+        <v>45657.57153850694</v>
       </c>
     </row>
     <row r="4">
@@ -658,13 +658,13 @@
         <v>42319</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.346527303317736e-67</v>
+        <v>-4.890623964652136e-79</v>
       </c>
       <c r="D4" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48926726852</v>
+        <v>45657.57153850694</v>
       </c>
     </row>
     <row r="5">
@@ -675,13 +675,13 @@
         <v>43057.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2300149811815606</v>
+        <v>-0.2300149801531476</v>
       </c>
       <c r="D5" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48926726852</v>
+        <v>45657.57153850694</v>
       </c>
     </row>
     <row r="6">
@@ -692,13 +692,13 @@
         <v>43355</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.2078946242637011</v>
+        <v>-0.2336519743029264</v>
       </c>
       <c r="D6" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45096.48926726852</v>
+        <v>45657.57153850694</v>
       </c>
     </row>
     <row r="7">
@@ -709,13 +709,13 @@
         <v>43719</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1152502200212455</v>
+        <v>-0.1376703730996233</v>
       </c>
       <c r="D7" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45096.48926726852</v>
+        <v>45657.57153850694</v>
       </c>
     </row>
     <row r="8">
@@ -726,13 +726,13 @@
         <v>44464.5</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.1041875609007215</v>
+        <v>-0.08124475998823612</v>
       </c>
       <c r="D8" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>45096.48926726852</v>
+        <v>45657.57153850694</v>
       </c>
     </row>
   </sheetData>
@@ -784,13 +784,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.04372244010723501</v>
+        <v>-0.04086481189390601</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48950741898</v>
+        <v>45657.57169365741</v>
       </c>
     </row>
     <row r="3">
@@ -801,13 +801,13 @@
         <v>42350.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0190716518511178</v>
+        <v>-0.03873412725521125</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48950741898</v>
+        <v>45657.57169365741</v>
       </c>
     </row>
     <row r="4">
@@ -818,13 +818,13 @@
         <v>43428.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.02219056568937188</v>
+        <v>-0.04412412725521125</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48950741898</v>
+        <v>45657.57169380787</v>
       </c>
     </row>
     <row r="5">
@@ -835,13 +835,13 @@
         <v>43792.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.02401056568937188</v>
+        <v>-0.0164932564953982</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.4895075926</v>
+        <v>45657.57169365741</v>
       </c>
     </row>
     <row r="6">
@@ -852,13 +852,13 @@
         <v>44807.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.302858935370898e-204</v>
+        <v>-4.674920645069725e-174</v>
       </c>
       <c r="D6" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45096.48950741898</v>
+        <v>45657.57169365741</v>
       </c>
     </row>
   </sheetData>
@@ -910,13 +910,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01545018607556224</v>
+        <v>-0.02256892312566483</v>
       </c>
       <c r="D2" t="n">
         <v>-1.17e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48980850694</v>
+        <v>45657.57188424769</v>
       </c>
     </row>
     <row r="3">
@@ -927,13 +927,13 @@
         <v>42049.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.02104873235195697</v>
+        <v>-0.02525560165766922</v>
       </c>
       <c r="D3" t="n">
         <v>-1.17e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48980850694</v>
+        <v>45657.57188424769</v>
       </c>
     </row>
     <row r="4">
@@ -944,13 +944,13 @@
         <v>43446</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0149920861385935</v>
+        <v>-0.01772351951977796</v>
       </c>
       <c r="D4" t="n">
         <v>-1.17e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48980850694</v>
+        <v>45657.57188424769</v>
       </c>
     </row>
     <row r="5">
@@ -961,13 +961,13 @@
         <v>43841.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.0196194361385935</v>
+        <v>-0.02235086951977796</v>
       </c>
       <c r="D5" t="n">
         <v>-1.17e-05</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48980870371</v>
+        <v>45657.57188435186</v>
       </c>
     </row>
   </sheetData>
@@ -1019,13 +1019,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2628918500032833</v>
+        <v>-0.3542975794951402</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48990774305</v>
+        <v>45657.57196103978</v>
       </c>
     </row>
     <row r="3">
@@ -1036,13 +1036,13 @@
         <v>41899</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.08153231183337238</v>
+        <v>-0.1426303880304105</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48990774305</v>
+        <v>45657.57196103978</v>
       </c>
     </row>
     <row r="4">
@@ -1053,13 +1053,13 @@
         <v>44104</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.119294298647568e-133</v>
+        <v>-1.02827751205387e-62</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48990774305</v>
+        <v>45657.57196103978</v>
       </c>
     </row>
     <row r="5">
@@ -1070,13 +1070,13 @@
         <v>44895</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-3.802005000714391e-57</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48990774305</v>
+        <v>45657.57196103978</v>
       </c>
     </row>
   </sheetData>
@@ -1697,13 +1697,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.02926255980664733</v>
+        <v>-0.0200142947273236</v>
       </c>
       <c r="D2" t="n">
         <v>-2.48e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48779674769</v>
+        <v>45657.57032079861</v>
       </c>
     </row>
     <row r="3">
@@ -1714,13 +1714,13 @@
         <v>43015.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.07850295980664732</v>
+        <v>-0.0692546947273236</v>
       </c>
       <c r="D3" t="n">
         <v>-2.48e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48779690972</v>
+        <v>45657.5703208912</v>
       </c>
     </row>
     <row r="4">
@@ -1731,13 +1731,13 @@
         <v>43467</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.05644296136702116</v>
+        <v>-0.04835544815926658</v>
       </c>
       <c r="D4" t="n">
         <v>-2.48e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48779674769</v>
+        <v>45657.57032079861</v>
       </c>
     </row>
     <row r="5">
@@ -1748,13 +1748,13 @@
         <v>44443.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.01548522604125567</v>
+        <v>-0.01629934320602976</v>
       </c>
       <c r="D5" t="n">
         <v>-2.48e-05</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48779674769</v>
+        <v>45657.57032079861</v>
       </c>
     </row>
   </sheetData>
@@ -2351,13 +2351,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.03979212470993771</v>
+        <v>-0.04136553704688054</v>
       </c>
       <c r="D2" t="n">
         <v>-1e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48796245371</v>
+        <v>45657.57041466435</v>
       </c>
     </row>
     <row r="3">
@@ -2368,13 +2368,13 @@
         <v>42707.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.01797319355054327</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D3" t="n">
         <v>-1e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48796245371</v>
+        <v>45657.57041466435</v>
       </c>
     </row>
     <row r="4">
@@ -2385,13 +2385,13 @@
         <v>44128.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.004752632617039575</v>
+        <v>-6.564079436993284e-147</v>
       </c>
       <c r="D4" t="n">
         <v>-1e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48796245371</v>
+        <v>45657.57041466435</v>
       </c>
     </row>
   </sheetData>
@@ -2443,13 +2443,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.07890387589317903</v>
+        <v>-0.0866734723037329</v>
       </c>
       <c r="D2" t="n">
         <v>-6e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48813849537</v>
+        <v>45657.57057532408</v>
       </c>
     </row>
     <row r="3">
@@ -2460,13 +2460,13 @@
         <v>41899</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.08411787589317903</v>
+        <v>-0.0918874723037329</v>
       </c>
       <c r="D3" t="n">
         <v>-6e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48813861111</v>
+        <v>45657.57057546296</v>
       </c>
     </row>
     <row r="4">
@@ -2477,13 +2477,13 @@
         <v>42987.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.09064887589317903</v>
+        <v>-0.09841847230373291</v>
       </c>
       <c r="D4" t="n">
         <v>-6e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48813861111</v>
+        <v>45657.57057546296</v>
       </c>
     </row>
     <row r="5">
@@ -2494,13 +2494,13 @@
         <v>44163.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.08544107047851823</v>
+        <v>-0.1054744723037329</v>
       </c>
       <c r="D5" t="n">
         <v>-6e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48813849537</v>
+        <v>45657.57057546296</v>
       </c>
     </row>
   </sheetData>
@@ -2552,13 +2552,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.04953366227438129</v>
+        <v>-0.06923117033577117</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48839530093</v>
+        <v>45657.57073831018</v>
       </c>
     </row>
     <row r="3">
@@ -2569,13 +2569,13 @@
         <v>42795</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.008237432704675522</v>
+        <v>-0.03393798164471695</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48839530093</v>
+        <v>45657.57073831018</v>
       </c>
     </row>
     <row r="4">
@@ -2586,13 +2586,13 @@
         <v>44079.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.01465993270467552</v>
+        <v>-0.04036048164471694</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48839552084</v>
+        <v>45657.57073841435</v>
       </c>
     </row>
     <row r="5">
@@ -2603,13 +2603,13 @@
         <v>44975.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.01913993270467552</v>
+        <v>-0.04484048164471695</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48839552084</v>
+        <v>45657.57073841435</v>
       </c>
     </row>
   </sheetData>
@@ -2661,13 +2661,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.05030037866555181</v>
+        <v>-0.007381263530535781</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48860040509</v>
+        <v>45657.57097861111</v>
       </c>
     </row>
     <row r="3">
@@ -2678,13 +2678,13 @@
         <v>42301.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.04643969981033326</v>
+        <v>-0.01373876353053578</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48860040509</v>
+        <v>45657.57097871528</v>
       </c>
     </row>
     <row r="4">
@@ -2695,13 +2695,13 @@
         <v>43386.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.05186469981033326</v>
+        <v>-0.01916376353053578</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.4886006713</v>
+        <v>45657.57097871528</v>
       </c>
     </row>
     <row r="5">
@@ -2712,13 +2712,13 @@
         <v>43750.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.03457768726041441</v>
+        <v>-0.008998939823900305</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48860040509</v>
+        <v>45657.57097861111</v>
       </c>
     </row>
     <row r="6">
@@ -2729,13 +2729,13 @@
         <v>44954.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.004798787091878788</v>
+        <v>-1e-08</v>
       </c>
       <c r="D6" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45096.48860040509</v>
+        <v>45657.57097861111</v>
       </c>
     </row>
   </sheetData>
@@ -2787,13 +2787,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-8.44236246457661e-146</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D2" t="n">
         <v>-0.0005</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48873192129</v>
+        <v>45657.57106283565</v>
       </c>
     </row>
     <row r="3">
@@ -2804,13 +2804,13 @@
         <v>42249</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.495079242664635e-205</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D3" t="n">
         <v>-0.0005</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48873192129</v>
+        <v>45657.57106283565</v>
       </c>
     </row>
     <row r="4">
@@ -2821,13 +2821,13 @@
         <v>43040</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1778185839198889</v>
+        <v>-0.1805246804431886</v>
       </c>
       <c r="D4" t="n">
         <v>-0.0005</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48873192129</v>
+        <v>45657.57106283565</v>
       </c>
     </row>
     <row r="5">
@@ -2838,13 +2838,13 @@
         <v>44499.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.03202589879324301</v>
+        <v>-8.08634922390439e-174</v>
       </c>
       <c r="D5" t="n">
         <v>-0.0005</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48873192129</v>
+        <v>45657.57106283565</v>
       </c>
     </row>
   </sheetData>
@@ -2896,13 +2896,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-6.067542711210391e-105</v>
+        <v>-8.478591186539953e-97</v>
       </c>
       <c r="D2" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48891115741</v>
+        <v>45657.57116181713</v>
       </c>
     </row>
     <row r="3">
@@ -2913,13 +2913,13 @@
         <v>41871</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.05987960134424146</v>
+        <v>-0.0600543450924556</v>
       </c>
       <c r="D3" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48891115741</v>
+        <v>45657.57116181713</v>
       </c>
     </row>
     <row r="4">
@@ -2930,13 +2930,13 @@
         <v>43082</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0793845257632721</v>
+        <v>-0.0003186787480661763</v>
       </c>
       <c r="D4" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48891115741</v>
+        <v>45657.57116181713</v>
       </c>
     </row>
     <row r="5">
@@ -2947,13 +2947,13 @@
         <v>44237</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1838839800477031</v>
+        <v>-0.04902615100419187</v>
       </c>
       <c r="D5" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48891115741</v>
+        <v>45657.57116181713</v>
       </c>
     </row>
   </sheetData>
@@ -3005,13 +3005,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.256754029630224e-28</v>
+        <v>-1.922848456476216e-30</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48905635416</v>
+        <v>45657.57132618056</v>
       </c>
     </row>
     <row r="3">
@@ -3022,13 +3022,13 @@
         <v>42655</v>
       </c>
       <c r="C3" t="n">
-        <v>-9.533384039595928e-28</v>
+        <v>-8.874685183736383e-29</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48905635416</v>
+        <v>45657.57132618056</v>
       </c>
     </row>
     <row r="4">
@@ -3045,7 +3045,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.4890566088</v>
+        <v>45657.57132628472</v>
       </c>
     </row>
     <row r="5">
@@ -3056,13 +3056,13 @@
         <v>43771.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.500204945252991e-29</v>
+        <v>-3.3526588471893e-30</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.48905635416</v>
+        <v>45657.57132618056</v>
       </c>
     </row>
     <row r="6">
@@ -3073,13 +3073,13 @@
         <v>44541.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-4.07462434764757e-26</v>
+        <v>-0.00385</v>
       </c>
       <c r="D6" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45096.48905635416</v>
+        <v>45657.57132628472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recomputed the results with the updated IKIEF data
</commit_message>
<xml_diff>
--- a/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
+++ b/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,13 +515,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.007945253551112148</v>
+        <v>-0.007945253565004884</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.49076744213</v>
+        <v>45659.67055324008</v>
       </c>
     </row>
     <row r="3">
@@ -532,13 +532,13 @@
         <v>42770.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-1.515419532809635e-128</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.49076744213</v>
+        <v>45659.67055324008</v>
       </c>
     </row>
     <row r="4">
@@ -549,13 +549,13 @@
         <v>43505.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-5.498708750262206e-115</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.49076744213</v>
+        <v>45659.67055324008</v>
       </c>
     </row>
     <row r="5">
@@ -566,13 +566,30 @@
         <v>43866</v>
       </c>
       <c r="C5" t="n">
-        <v>-2.240216970902034e-116</v>
+        <v>-1.688318500038388e-108</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.49076744213</v>
+        <v>45659.67055324008</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>45304.5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.003332480416235479</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>45659.67055324008</v>
       </c>
     </row>
   </sheetData>
@@ -624,13 +641,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.148933078226618e-72</v>
+        <v>-6.565340830236557e-72</v>
       </c>
       <c r="D2" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57153850694</v>
+        <v>45659.66882101852</v>
       </c>
     </row>
     <row r="3">
@@ -638,16 +655,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>41682</v>
+        <v>42319</v>
       </c>
       <c r="C3" t="n">
-        <v>-7.373037232174746e-77</v>
+        <v>-1.936106931141733e-68</v>
       </c>
       <c r="D3" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57153850694</v>
+        <v>45659.66882101852</v>
       </c>
     </row>
     <row r="4">
@@ -655,16 +672,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>42319</v>
+        <v>43057.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.890623964652136e-79</v>
+        <v>-0.2300149888669734</v>
       </c>
       <c r="D4" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57153850694</v>
+        <v>45659.66882101852</v>
       </c>
     </row>
     <row r="5">
@@ -672,16 +689,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>43057.5</v>
+        <v>43355</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2300149801531476</v>
+        <v>-0.2336519701827103</v>
       </c>
       <c r="D5" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45657.57153850694</v>
+        <v>45659.66882101852</v>
       </c>
     </row>
     <row r="6">
@@ -689,16 +706,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>43355</v>
+        <v>43719</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.2336519743029264</v>
+        <v>-0.1376703607037062</v>
       </c>
       <c r="D6" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45657.57153850694</v>
+        <v>45659.66882101852</v>
       </c>
     </row>
     <row r="7">
@@ -706,16 +723,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>43719</v>
+        <v>44464.5</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1376703730996233</v>
+        <v>-0.155412431132807</v>
       </c>
       <c r="D7" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45657.57153850694</v>
+        <v>45659.66882101852</v>
       </c>
     </row>
     <row r="8">
@@ -723,16 +740,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>44464.5</v>
+        <v>45224</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.08124475998823612</v>
+        <v>-0.1921928980098065</v>
       </c>
       <c r="D8" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>45657.57153850694</v>
+        <v>45659.66882101852</v>
       </c>
     </row>
   </sheetData>
@@ -790,7 +807,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57169365741</v>
+        <v>45659.66904085648</v>
       </c>
     </row>
     <row r="3">
@@ -807,7 +824,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57169365741</v>
+        <v>45659.66904085648</v>
       </c>
     </row>
     <row r="4">
@@ -824,7 +841,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57169380787</v>
+        <v>45659.6690409838</v>
       </c>
     </row>
     <row r="5">
@@ -841,7 +858,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45657.57169365741</v>
+        <v>45659.66904085648</v>
       </c>
     </row>
     <row r="6">
@@ -858,7 +875,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45657.57169365741</v>
+        <v>45659.66904085648</v>
       </c>
     </row>
   </sheetData>
@@ -916,7 +933,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57188424769</v>
+        <v>45659.66927358796</v>
       </c>
     </row>
     <row r="3">
@@ -933,7 +950,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57188424769</v>
+        <v>45659.66927358796</v>
       </c>
     </row>
     <row r="4">
@@ -950,7 +967,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57188424769</v>
+        <v>45659.66927358796</v>
       </c>
     </row>
     <row r="5">
@@ -967,7 +984,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45657.57188435186</v>
+        <v>45659.66927394676</v>
       </c>
     </row>
   </sheetData>
@@ -981,7 +998,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1019,13 +1036,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.3542975794951402</v>
+        <v>-0.2052437387740799</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57196103978</v>
+        <v>45659.66935649305</v>
       </c>
     </row>
     <row r="3">
@@ -1033,16 +1050,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>41899</v>
+        <v>44104</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1426303880304105</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57196103978</v>
+        <v>45659.66935649305</v>
       </c>
     </row>
     <row r="4">
@@ -1050,33 +1067,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44104</v>
+        <v>44895</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.02827751205387e-62</v>
+        <v>-5.390931173173605e-79</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57196103978</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>44895</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-3.802005000714391e-57</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>45657.57196103978</v>
+        <v>45659.66935649305</v>
       </c>
     </row>
   </sheetData>
@@ -1128,13 +1128,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1184799798297854</v>
+        <v>-0.1184799810075869</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.48995410879</v>
+        <v>45659.66939689815</v>
       </c>
     </row>
     <row r="3">
@@ -1145,13 +1145,13 @@
         <v>43085.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.291988874337228e-19</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.48995410879</v>
+        <v>45659.66939689815</v>
       </c>
     </row>
     <row r="4">
@@ -1162,13 +1162,13 @@
         <v>45003.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-1e-08</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.48995410879</v>
+        <v>45659.66939689815</v>
       </c>
     </row>
   </sheetData>
@@ -1220,13 +1220,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.002171265363407897</v>
+        <v>-4.921843761759291e-13</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.49000885417</v>
+        <v>45659.66943119213</v>
       </c>
     </row>
     <row r="3">
@@ -1234,16 +1234,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>43446</v>
+        <v>44146</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.004736696322308073</v>
+        <v>-0.008432500000492185</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.49000885417</v>
+        <v>45659.66943126157</v>
       </c>
     </row>
     <row r="4">
@@ -1251,16 +1251,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44146</v>
+        <v>45346.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.008236696322308073</v>
+        <v>-1e-08</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.49000898148</v>
+        <v>45659.66943119213</v>
       </c>
     </row>
   </sheetData>
@@ -1312,13 +1312,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.002949466042271664</v>
+        <v>-0.004725025682886591</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.49013689814</v>
+        <v>45659.66952358796</v>
       </c>
     </row>
     <row r="3">
@@ -1329,13 +1329,13 @@
         <v>43533.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.008319466042271665</v>
+        <v>-0.01009502568288659</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.49013703704</v>
+        <v>45659.66952368055</v>
       </c>
     </row>
     <row r="4">
@@ -1346,13 +1346,13 @@
         <v>43897.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.01013946604227166</v>
+        <v>-0.01191502568288659</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.49013703704</v>
+        <v>45659.66952368055</v>
       </c>
     </row>
     <row r="5">
@@ -1363,13 +1363,13 @@
         <v>44569.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-9.571012963945394e-19</v>
+        <v>-5.275102230893418e-38</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.49013689814</v>
+        <v>45659.66952358796</v>
       </c>
     </row>
     <row r="6">
@@ -1380,13 +1380,13 @@
         <v>44912.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-1e-08</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D6" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45096.49013689814</v>
+        <v>45659.66952358796</v>
       </c>
     </row>
   </sheetData>
@@ -1400,7 +1400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1438,13 +1438,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01859569388601449</v>
+        <v>-0.01593374205496519</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.4902321412</v>
+        <v>45659.66957560185</v>
       </c>
     </row>
     <row r="3">
@@ -1452,16 +1452,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>43141.5</v>
+        <v>44268.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.02200569388601449</v>
+        <v>-0.02497874205496519</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.49023223379</v>
+        <v>45659.66957570602</v>
       </c>
     </row>
     <row r="4">
@@ -1469,33 +1469,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44268.5</v>
+        <v>44611.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.02764069388601449</v>
+        <v>-1.131086630713581e-70</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.49023223379</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>44611.5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-5.081170449047601e-262</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>45096.4902321412</v>
+        <v>45659.66957560185</v>
       </c>
     </row>
   </sheetData>
@@ -1509,7 +1492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1547,13 +1530,30 @@
         <v>43991.54166666666</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.001262099947825627</v>
+        <v>-0.00126209991859047</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.49025758102</v>
+        <v>45659.66961061343</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>45325.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1e-08</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>45659.66961061343</v>
       </c>
     </row>
   </sheetData>
@@ -1605,13 +1605,13 @@
         <v>42461.45833333334</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1545491158101825</v>
+        <v>-0.15454911616953</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.49029898148</v>
+        <v>45659.66965627314</v>
       </c>
     </row>
     <row r="3">
@@ -1622,13 +1622,13 @@
         <v>42637.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1554293241435159</v>
+        <v>-0.1554293245028633</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.49029907407</v>
+        <v>45659.66965637731</v>
       </c>
     </row>
     <row r="4">
@@ -1639,13 +1639,13 @@
         <v>44170.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.07961501487479707</v>
+        <v>-0.103399979231424</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.49029898148</v>
+        <v>45659.66965627314</v>
       </c>
     </row>
   </sheetData>
@@ -1654,6 +1654,98 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>datum</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>offset</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>slope</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>gewijzigd</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>41030</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-0.01200912636030523</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-2.48e-05</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>45659.66733104167</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>43015.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.06114951240814359</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-2.48e-05</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>45659.66733104167</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>44443.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.01629934187726835</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-2.48e-05</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45659.66733104167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1694,16 +1786,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>41030</v>
+        <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0200142947273236</v>
+        <v>-0.1044418001850728</v>
       </c>
       <c r="D2" t="n">
-        <v>-2.48e-05</v>
+        <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57032079861</v>
+        <v>45659.66972641204</v>
       </c>
     </row>
     <row r="3">
@@ -1711,16 +1803,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>43015.5</v>
+        <v>43120.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0692546947273236</v>
+        <v>-0.1077468001850728</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.48e-05</v>
+        <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.5703208912</v>
+        <v>45659.66972648148</v>
       </c>
     </row>
     <row r="4">
@@ -1728,16 +1820,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>43467</v>
+        <v>44590.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.04835544815926658</v>
+        <v>-0.1150968001850728</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.48e-05</v>
+        <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57032079861</v>
+        <v>45659.66972648148</v>
       </c>
     </row>
     <row r="5">
@@ -1745,16 +1837,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>44443.5</v>
+        <v>45241.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.01629934320602976</v>
+        <v>-0.007458571015559286</v>
       </c>
       <c r="D5" t="n">
-        <v>-2.48e-05</v>
+        <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45657.57032079861</v>
+        <v>45659.66972641204</v>
       </c>
     </row>
   </sheetData>
@@ -1762,7 +1854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1806,13 +1898,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1022601204382361</v>
+        <v>-1.432766686621208e-10</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.49035333333</v>
+        <v>45659.66974891203</v>
       </c>
     </row>
     <row r="3">
@@ -1820,16 +1912,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>43120.5</v>
+        <v>44044.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1055651204382361</v>
+        <v>-1.432072678524741e-10</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.4903534375</v>
+        <v>45659.66974891203</v>
       </c>
     </row>
     <row r="4">
@@ -1837,16 +1929,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44590.5</v>
+        <v>44520.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1129151204382361</v>
+        <v>-1.687511798234804e-05</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.4903534375</v>
+        <v>45659.66974891203</v>
       </c>
     </row>
   </sheetData>
@@ -1854,7 +1946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1898,13 +1990,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.006533887873377515</v>
+        <v>-1.618228381013169e-13</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.4904037963</v>
+        <v>45659.66986012732</v>
       </c>
     </row>
     <row r="3">
@@ -1912,16 +2004,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>43190.5</v>
+        <v>43141.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-0.003410000000161823</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.4904037963</v>
+        <v>45659.66986023148</v>
       </c>
     </row>
     <row r="4">
@@ -1929,16 +2021,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44044.5</v>
+        <v>44202</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-0.008712500000161825</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.4904037963</v>
+        <v>45659.66986023148</v>
       </c>
     </row>
     <row r="5">
@@ -1946,16 +2038,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>44520.5</v>
+        <v>44258</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-0.008992500000161824</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.4904037963</v>
+        <v>45659.66986023148</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +2055,99 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>datum</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>offset</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>slope</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>gewijzigd</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>42461.45833333334</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1.072784857913832e-73</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>45659.66988943287</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>43169.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-4.940656458412465e-324</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>45659.66988943287</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>44933.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.007396293739223675</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45659.66988943287</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2007,13 +2191,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.00345728343297063</v>
+        <v>-8.880238603714169e-16</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45096.49057321759</v>
+        <v>45659.67051150463</v>
       </c>
     </row>
     <row r="3">
@@ -2021,16 +2205,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>43141.5</v>
+        <v>42679.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.006867283432970631</v>
+        <v>-3.422840394731303e-16</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45096.49057332176</v>
+        <v>45659.67051150463</v>
       </c>
     </row>
     <row r="4">
@@ -2038,16 +2222,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>43502</v>
+        <v>44286</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.00866978343297063</v>
+        <v>-0.008032500000000343</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45096.49057332176</v>
+        <v>45659.67051181713</v>
       </c>
     </row>
     <row r="5">
@@ -2055,16 +2239,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>44202</v>
+        <v>44849.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.01216978343297063</v>
+        <v>-1e-08</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45096.49057332176</v>
+        <v>45659.67051150463</v>
       </c>
     </row>
     <row r="6">
@@ -2072,234 +2256,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>44258</v>
+        <v>45269.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.01244978343297063</v>
+        <v>-2.968811667670847e-16</v>
       </c>
       <c r="D6" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45096.49057332176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>datum</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>offset</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>slope</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>gewijzigd</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>42461.45833333334</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-7.502716848988574e-15</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>45096.49059289352</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>43169.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-1e-08</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>45096.49059289352</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>43537</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-1.625301915072294e-14</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45096.49059289352</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>44933.5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-1e-08</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>45096.49059289352</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>datum</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>offset</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>slope</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>gewijzigd</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>42459.5</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-6.458576972480369e-16</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>45096.49073003473</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>42679.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-0.001100000000000646</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>45096.49073011574</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>44286</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-0.009132500000000645</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45096.49073011574</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>44849.5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-1e-08</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>45096.49073003473</v>
+        <v>45659.67051150463</v>
       </c>
     </row>
   </sheetData>
@@ -2357,7 +2323,7 @@
         <v>-1e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57041466435</v>
+        <v>45659.66746710648</v>
       </c>
     </row>
     <row r="3">
@@ -2374,7 +2340,7 @@
         <v>-1e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57041466435</v>
+        <v>45659.66746710648</v>
       </c>
     </row>
     <row r="4">
@@ -2391,7 +2357,7 @@
         <v>-1e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57041466435</v>
+        <v>45659.66746710648</v>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2449,7 +2415,7 @@
         <v>-6e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57057532408</v>
+        <v>45659.66764652778</v>
       </c>
     </row>
     <row r="3">
@@ -2457,16 +2423,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>41899</v>
+        <v>42987.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0918874723037329</v>
+        <v>-0.09841847230373291</v>
       </c>
       <c r="D3" t="n">
         <v>-6e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57057546296</v>
+        <v>45659.66764662037</v>
       </c>
     </row>
     <row r="4">
@@ -2474,33 +2440,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>42987.5</v>
+        <v>44163.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.09841847230373291</v>
+        <v>-0.1054744723037329</v>
       </c>
       <c r="D4" t="n">
         <v>-6e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57057546296</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>44163.5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-0.1054744723037329</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-6e-06</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>45657.57057546296</v>
+        <v>45659.66764662037</v>
       </c>
     </row>
   </sheetData>
@@ -2558,7 +2507,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57073831018</v>
+        <v>45659.66787927083</v>
       </c>
     </row>
     <row r="3">
@@ -2575,7 +2524,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57073831018</v>
+        <v>45659.66787927083</v>
       </c>
     </row>
     <row r="4">
@@ -2592,7 +2541,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57073841435</v>
+        <v>45659.66787939815</v>
       </c>
     </row>
     <row r="5">
@@ -2609,7 +2558,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45657.57073841435</v>
+        <v>45659.66787939815</v>
       </c>
     </row>
   </sheetData>
@@ -2667,7 +2616,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57097861111</v>
+        <v>45659.66819157408</v>
       </c>
     </row>
     <row r="3">
@@ -2684,7 +2633,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57097871528</v>
+        <v>45659.66819166666</v>
       </c>
     </row>
     <row r="4">
@@ -2701,7 +2650,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57097871528</v>
+        <v>45659.66819166666</v>
       </c>
     </row>
     <row r="5">
@@ -2718,7 +2667,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45657.57097861111</v>
+        <v>45659.66819157408</v>
       </c>
     </row>
     <row r="6">
@@ -2735,7 +2684,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45657.57097861111</v>
+        <v>45659.66819157408</v>
       </c>
     </row>
   </sheetData>
@@ -2749,7 +2698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2793,7 +2742,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57106283565</v>
+        <v>45659.6683221412</v>
       </c>
     </row>
     <row r="3">
@@ -2810,7 +2759,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57106283565</v>
+        <v>45659.6683221412</v>
       </c>
     </row>
     <row r="4">
@@ -2821,13 +2770,13 @@
         <v>43040</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1805246804431886</v>
+        <v>-0.1805246675845648</v>
       </c>
       <c r="D4" t="n">
         <v>-0.0005</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57106283565</v>
+        <v>45659.6683221412</v>
       </c>
     </row>
     <row r="5">
@@ -2838,13 +2787,30 @@
         <v>44499.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-8.08634922390439e-174</v>
+        <v>-0.1547357292117479</v>
       </c>
       <c r="D5" t="n">
         <v>-0.0005</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45657.57106283565</v>
+        <v>45659.6683221412</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>45178.5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.04881652716562163</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.0005</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>45659.6683221412</v>
       </c>
     </row>
   </sheetData>
@@ -2858,7 +2824,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2896,13 +2862,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-8.478591186539953e-97</v>
+        <v>-1.678513233955944e-114</v>
       </c>
       <c r="D2" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57116181713</v>
+        <v>45659.66842271991</v>
       </c>
     </row>
     <row r="3">
@@ -2910,16 +2876,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>41871</v>
+        <v>44237</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0600543450924556</v>
+        <v>-0.115114525930587</v>
       </c>
       <c r="D3" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57116181713</v>
+        <v>45659.66842271991</v>
       </c>
     </row>
     <row r="4">
@@ -2927,33 +2893,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>43082</v>
+        <v>45203</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0003186787480661763</v>
+        <v>-0.1442103368313238</v>
       </c>
       <c r="D4" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57116181713</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>44237</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-0.04902615100419187</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.0003</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>45657.57116181713</v>
+        <v>45659.66842271991</v>
       </c>
     </row>
   </sheetData>
@@ -3011,7 +2960,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45657.57132618056</v>
+        <v>45659.66861936342</v>
       </c>
     </row>
     <row r="3">
@@ -3028,7 +2977,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45657.57132618056</v>
+        <v>45659.66861936342</v>
       </c>
     </row>
     <row r="4">
@@ -3045,7 +2994,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45657.57132628472</v>
+        <v>45659.66861947917</v>
       </c>
     </row>
     <row r="5">
@@ -3062,7 +3011,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45657.57132618056</v>
+        <v>45659.66861936342</v>
       </c>
     </row>
     <row r="6">
@@ -3079,7 +3028,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45657.57132628472</v>
+        <v>45659.66861947917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update coefficients for 2025 report
</commit_message>
<xml_diff>
--- a/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
+++ b/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
@@ -521,7 +521,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.67055324008</v>
+        <v>45693.44442742501</v>
       </c>
     </row>
     <row r="3">
@@ -538,7 +538,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.67055324008</v>
+        <v>45693.44442742501</v>
       </c>
     </row>
     <row r="4">
@@ -555,7 +555,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.67055324008</v>
+        <v>45693.44442742501</v>
       </c>
     </row>
     <row r="5">
@@ -572,7 +572,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.67055324008</v>
+        <v>45693.44442742501</v>
       </c>
     </row>
     <row r="6">
@@ -589,7 +589,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45659.67055324008</v>
+        <v>45693.44442742501</v>
       </c>
     </row>
   </sheetData>
@@ -603,7 +603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,13 +641,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-6.565340830236557e-72</v>
+        <v>-9.441419276088441e-69</v>
       </c>
       <c r="D2" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66882101852</v>
+        <v>45693.44323549768</v>
       </c>
     </row>
     <row r="3">
@@ -658,13 +658,13 @@
         <v>42319</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.936106931141733e-68</v>
+        <v>-4.611154693734719e-66</v>
       </c>
       <c r="D3" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66882101852</v>
+        <v>45693.44323549768</v>
       </c>
     </row>
     <row r="4">
@@ -675,13 +675,13 @@
         <v>43057.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.2300149888669734</v>
+        <v>-0.258475</v>
       </c>
       <c r="D4" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66882101852</v>
+        <v>45693.44323569445</v>
       </c>
     </row>
     <row r="5">
@@ -692,13 +692,13 @@
         <v>43355</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2336519701827103</v>
+        <v>-0.3626</v>
       </c>
       <c r="D5" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.66882101852</v>
+        <v>45693.44323569445</v>
       </c>
     </row>
     <row r="6">
@@ -706,16 +706,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>43719</v>
+        <v>43418</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.1376703607037062</v>
+        <v>-0.1035954282753379</v>
       </c>
       <c r="D6" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45659.66882101852</v>
+        <v>45693.44323549768</v>
       </c>
     </row>
     <row r="7">
@@ -723,16 +723,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>44464.5</v>
+        <v>43719</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.155412431132807</v>
+        <v>-0.137670349791598</v>
       </c>
       <c r="D7" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45659.66882101852</v>
+        <v>45693.44323549768</v>
       </c>
     </row>
     <row r="8">
@@ -740,16 +740,33 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>45224</v>
+        <v>44464.5</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.1921928980098065</v>
+        <v>-0.1554124289160655</v>
       </c>
       <c r="D8" t="n">
         <v>-0.00035</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>45659.66882101852</v>
+        <v>45693.44323549768</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>45224</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.1921929130604666</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.00035</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>45693.44323549768</v>
       </c>
     </row>
   </sheetData>
@@ -807,7 +824,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66904085648</v>
+        <v>45693.44338636574</v>
       </c>
     </row>
     <row r="3">
@@ -824,7 +841,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66904085648</v>
+        <v>45693.44338636574</v>
       </c>
     </row>
     <row r="4">
@@ -841,7 +858,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.6690409838</v>
+        <v>45693.44338651621</v>
       </c>
     </row>
     <row r="5">
@@ -858,7 +875,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.66904085648</v>
+        <v>45693.44338636574</v>
       </c>
     </row>
     <row r="6">
@@ -875,7 +892,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45659.66904085648</v>
+        <v>45693.44338636574</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +950,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66927358796</v>
+        <v>45693.44357704861</v>
       </c>
     </row>
     <row r="3">
@@ -950,7 +967,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66927358796</v>
+        <v>45693.44357704861</v>
       </c>
     </row>
     <row r="4">
@@ -967,7 +984,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66927358796</v>
+        <v>45693.44357704861</v>
       </c>
     </row>
     <row r="5">
@@ -984,7 +1001,7 @@
         <v>-1.17e-05</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.66927394676</v>
+        <v>45693.44357719908</v>
       </c>
     </row>
   </sheetData>
@@ -998,7 +1015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1036,13 +1053,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2052437387740799</v>
+        <v>-0.2424197781309921</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66935649305</v>
+        <v>45693.44365953704</v>
       </c>
     </row>
     <row r="3">
@@ -1050,16 +1067,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>44104</v>
+        <v>43068</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-0.04013794385646279</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66935649305</v>
+        <v>45693.44365953704</v>
       </c>
     </row>
     <row r="4">
@@ -1067,16 +1084,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-4.940656458412465e-324</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45693.44365953704</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>44895</v>
       </c>
-      <c r="C4" t="n">
-        <v>-5.390931173173605e-79</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45659.66935649305</v>
+      <c r="C5" t="n">
+        <v>-4.556301014564934e-210</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44365953704</v>
       </c>
     </row>
   </sheetData>
@@ -1090,7 +1124,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1128,13 +1162,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1184799810075869</v>
+        <v>-0.1184799807480392</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66939689815</v>
+        <v>45693.44370694445</v>
       </c>
     </row>
     <row r="3">
@@ -1145,13 +1179,13 @@
         <v>43085.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-1e-08</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66939689815</v>
+        <v>45693.44370694445</v>
       </c>
     </row>
     <row r="4">
@@ -1159,16 +1193,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
+        <v>43470.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.0008229490695431941</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45693.44370694445</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>45003.5</v>
       </c>
-      <c r="C4" t="n">
-        <v>-4.940656458412465e-324</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45659.66939689815</v>
+      <c r="C5" t="n">
+        <v>-1.125452894031154e-12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44370694445</v>
       </c>
     </row>
   </sheetData>
@@ -1182,7 +1233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1220,13 +1271,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-4.921843761759291e-13</v>
+        <v>-0.002171277797143856</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66943119213</v>
+        <v>45693.44375903935</v>
       </c>
     </row>
     <row r="3">
@@ -1234,16 +1285,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>44146</v>
+        <v>43446</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.008432500000492185</v>
+        <v>-0.004736695874612127</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66943126157</v>
+        <v>45693.44375903935</v>
       </c>
     </row>
     <row r="4">
@@ -1251,16 +1302,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
+        <v>44146</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.008236695874612126</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45693.44375912037</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>45346.5</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>-1e-08</v>
       </c>
-      <c r="D4" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45659.66943119213</v>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44375903935</v>
       </c>
     </row>
   </sheetData>
@@ -1318,7 +1386,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66952358796</v>
+        <v>45693.44384069445</v>
       </c>
     </row>
     <row r="3">
@@ -1335,7 +1403,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66952368055</v>
+        <v>45693.44384082176</v>
       </c>
     </row>
     <row r="4">
@@ -1352,7 +1420,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66952368055</v>
+        <v>45693.44384082176</v>
       </c>
     </row>
     <row r="5">
@@ -1369,7 +1437,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.66952358796</v>
+        <v>45693.44384069445</v>
       </c>
     </row>
     <row r="6">
@@ -1386,7 +1454,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45659.66952358796</v>
+        <v>45693.44384069445</v>
       </c>
     </row>
   </sheetData>
@@ -1400,7 +1468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1444,7 +1512,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66957560185</v>
+        <v>45693.44391109954</v>
       </c>
     </row>
     <row r="3">
@@ -1452,16 +1520,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>44268.5</v>
+        <v>43152</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.02497874205496519</v>
+        <v>-0.01939624205496519</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66957570602</v>
+        <v>45693.44391116898</v>
       </c>
     </row>
     <row r="4">
@@ -1469,16 +1537,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
+        <v>44268.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.02497874205496519</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45693.44391116898</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>44611.5</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>-1.131086630713581e-70</v>
       </c>
-      <c r="D4" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45659.66957560185</v>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44391109954</v>
       </c>
     </row>
   </sheetData>
@@ -1536,7 +1621,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66961061343</v>
+        <v>45693.44394638889</v>
       </c>
     </row>
     <row r="3">
@@ -1553,7 +1638,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66961061343</v>
+        <v>45693.44394638889</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1696,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66965627314</v>
+        <v>45693.44398280093</v>
       </c>
     </row>
     <row r="3">
@@ -1628,7 +1713,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66965637731</v>
+        <v>45693.44398287037</v>
       </c>
     </row>
     <row r="4">
@@ -1645,7 +1730,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66965627314</v>
+        <v>45693.44398280093</v>
       </c>
     </row>
   </sheetData>
@@ -1659,7 +1744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1697,13 +1782,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01200912636030523</v>
+        <v>-0.02001429472706926</v>
       </c>
       <c r="D2" t="n">
         <v>-2.48e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66733104167</v>
+        <v>45693.4416002662</v>
       </c>
     </row>
     <row r="3">
@@ -1714,13 +1799,13 @@
         <v>43015.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.06114951240814359</v>
+        <v>-0.06925469472706926</v>
       </c>
       <c r="D3" t="n">
         <v>-2.48e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66733104167</v>
+        <v>45693.4416003588</v>
       </c>
     </row>
     <row r="4">
@@ -1728,16 +1813,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44443.5</v>
+        <v>43390</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.01629934187726835</v>
+        <v>-0.04644584477735266</v>
       </c>
       <c r="D4" t="n">
         <v>-2.48e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66733104167</v>
+        <v>45693.4416002662</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>44443.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.01629934319962626</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-2.48e-05</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.4416002662</v>
       </c>
     </row>
   </sheetData>
@@ -1795,7 +1897,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66972641204</v>
+        <v>45693.44404040509</v>
       </c>
     </row>
     <row r="3">
@@ -1812,7 +1914,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66972648148</v>
+        <v>45693.44404047454</v>
       </c>
     </row>
     <row r="4">
@@ -1829,7 +1931,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66972648148</v>
+        <v>45693.44404047454</v>
       </c>
     </row>
     <row r="5">
@@ -1846,7 +1948,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.66972641204</v>
+        <v>45693.44404040509</v>
       </c>
     </row>
   </sheetData>
@@ -1855,98 +1957,6 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>datum</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>offset</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>slope</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>gewijzigd</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>42459.5</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-1.432766686621208e-10</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>45659.66974891203</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>44044.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-1.432072678524741e-10</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>45659.66974891203</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>44520.5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-1.687511798234804e-05</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45659.66974891203</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1990,13 +2000,13 @@
         <v>42459.5</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.618228381013169e-13</v>
+        <v>-0.005762739932864545</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66986012732</v>
+        <v>45693.44408138889</v>
       </c>
     </row>
     <row r="3">
@@ -2004,16 +2014,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>43141.5</v>
+        <v>43173</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.003410000000161823</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66986023148</v>
+        <v>45693.44408138889</v>
       </c>
     </row>
     <row r="4">
@@ -2021,16 +2031,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44202</v>
+        <v>44044.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.008712500000161825</v>
+        <v>-4.940656458412465e-324</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66986023148</v>
+        <v>45693.44408138889</v>
       </c>
     </row>
     <row r="5">
@@ -2038,16 +2048,159 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="n">
+        <v>44520.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-3.431319654256471e-05</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44408138889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>datum</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>offset</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>slope</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>gewijzigd</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>42459.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1.618228381013169e-13</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>45693.4442225</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>43141.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.003410000000161823</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>45693.44422258102</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>43509</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.005247500000161823</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45693.44422258102</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>44202</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.008712500000161825</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44422258102</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="n">
         <v>44258</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C6" t="n">
         <v>-0.008992500000161824</v>
       </c>
-      <c r="D5" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>45659.66986023148</v>
+      <c r="D6" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>45693.44422258102</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>44545</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.01042750000016182</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>45693.44422258102</v>
       </c>
     </row>
   </sheetData>
@@ -2061,7 +2214,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2099,13 +2252,13 @@
         <v>42461.45833333334</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.072784857913832e-73</v>
+        <v>-3.318272141960634e-08</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66988943287</v>
+        <v>45693.44425013889</v>
       </c>
     </row>
     <row r="3">
@@ -2116,13 +2269,13 @@
         <v>43169.5</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.940656458412465e-324</v>
+        <v>-1e-08</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66988943287</v>
+        <v>45693.44425013889</v>
       </c>
     </row>
     <row r="4">
@@ -2130,16 +2283,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
+        <v>43537</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-4.543592561502216e-38</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45693.44425013889</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>44933.5</v>
       </c>
-      <c r="C4" t="n">
-        <v>-0.007396293739223675</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45659.66988943287</v>
+      <c r="C5" t="n">
+        <v>-0.006729508378068172</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44425013889</v>
       </c>
     </row>
   </sheetData>
@@ -2148,6 +2318,149 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>datum</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>offset</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>slope</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>gewijzigd</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>42459.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1.022742258970684e-14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>45693.44439063657</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>42679.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1.754831467298821e-12</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>45693.44439063657</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>43047</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.00180171220572806</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>45693.44439063657</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.007996712205728061</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44439076389</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>44849.5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1e-08</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>45693.44439063657</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>45269.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-9.891230824199055e-154</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>45693.44439063657</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2188,16 +2501,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>42459.5</v>
+        <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-8.880238603714169e-16</v>
+        <v>-0.04136553504106202</v>
       </c>
       <c r="D2" t="n">
-        <v>-5e-06</v>
+        <v>-1e-05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.67051150463</v>
+        <v>45693.4418258912</v>
       </c>
     </row>
     <row r="3">
@@ -2205,16 +2518,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>42679.5</v>
+        <v>41640</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.422840394731303e-16</v>
+        <v>-0.04746553504106202</v>
       </c>
       <c r="D3" t="n">
-        <v>-5e-06</v>
+        <v>-1e-05</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.67051150463</v>
+        <v>45693.44182601852</v>
       </c>
     </row>
     <row r="4">
@@ -2222,16 +2535,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44286</v>
+        <v>42707.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.008032500000000343</v>
+        <v>-1.714892393715332e-59</v>
       </c>
       <c r="D4" t="n">
-        <v>-5e-06</v>
+        <v>-1e-05</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.67051181713</v>
+        <v>45693.4418258912</v>
       </c>
     </row>
     <row r="5">
@@ -2239,16 +2552,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>44849.5</v>
+        <v>43026</v>
       </c>
       <c r="C5" t="n">
-        <v>-1e-08</v>
+        <v>-3.267571342321195e-62</v>
       </c>
       <c r="D5" t="n">
-        <v>-5e-06</v>
+        <v>-1e-05</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.67051150463</v>
+        <v>45693.4418258912</v>
       </c>
     </row>
     <row r="6">
@@ -2256,108 +2569,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>45269.5</v>
+        <v>44128.5</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.968811667670847e-16</v>
+        <v>-1.037013949096437e-55</v>
       </c>
       <c r="D6" t="n">
-        <v>-5e-06</v>
+        <v>-1e-05</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45659.67051150463</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>datum</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>offset</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>slope</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>gewijzigd</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>41030</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-0.04136553704688054</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-1e-05</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>45659.66746710648</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>42707.5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-4.940656458412465e-324</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-1e-05</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>45659.66746710648</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>44128.5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-6.564079436993284e-147</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-1e-05</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>45659.66746710648</v>
+        <v>45693.4418258912</v>
       </c>
     </row>
   </sheetData>
@@ -2371,7 +2592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2415,7 +2636,7 @@
         <v>-6e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66764652778</v>
+        <v>45693.44204214121</v>
       </c>
     </row>
     <row r="3">
@@ -2423,16 +2644,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>42987.5</v>
+        <v>41941</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.09841847230373291</v>
+        <v>-0.0921394723037329</v>
       </c>
       <c r="D3" t="n">
         <v>-6e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66764662037</v>
+        <v>45693.44204222222</v>
       </c>
     </row>
     <row r="4">
@@ -2440,16 +2661,50 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44163.5</v>
+        <v>42987.5</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1054744723037329</v>
+        <v>-0.09841847230373291</v>
       </c>
       <c r="D4" t="n">
         <v>-6e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66764662037</v>
+        <v>45693.44204222222</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>43355</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.1006234723037329</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-6e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44204222222</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>44163.5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.1054744723037329</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-6e-06</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>45693.44204222222</v>
       </c>
     </row>
   </sheetData>
@@ -2463,7 +2718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2501,13 +2756,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.06923117033577117</v>
+        <v>-0.09901636173436058</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66787927083</v>
+        <v>45693.44223667824</v>
       </c>
     </row>
     <row r="3">
@@ -2515,16 +2770,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>42795</v>
+        <v>41794</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.03393798164471695</v>
+        <v>-0.04295056884621479</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66787927083</v>
+        <v>45693.44223667824</v>
       </c>
     </row>
     <row r="4">
@@ -2532,16 +2787,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>44079.5</v>
+        <v>42795</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.04036048164471694</v>
+        <v>-0.03393798179998574</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66787939815</v>
+        <v>45693.44223667824</v>
       </c>
     </row>
     <row r="5">
@@ -2549,16 +2804,33 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="n">
+        <v>44079.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.04036048179998574</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45693.44223694444</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="n">
         <v>44975.5</v>
       </c>
-      <c r="C5" t="n">
-        <v>-0.04484048164471695</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>45659.66787939815</v>
+      <c r="C6" t="n">
+        <v>-0.04484048179998575</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>45693.44223694444</v>
       </c>
     </row>
   </sheetData>
@@ -2616,7 +2888,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66819157408</v>
+        <v>45693.44248314814</v>
       </c>
     </row>
     <row r="3">
@@ -2633,7 +2905,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66819166666</v>
+        <v>45693.44248324074</v>
       </c>
     </row>
     <row r="4">
@@ -2650,7 +2922,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66819166666</v>
+        <v>45693.44248324074</v>
       </c>
     </row>
     <row r="5">
@@ -2667,7 +2939,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.66819157408</v>
+        <v>45693.44248314814</v>
       </c>
     </row>
     <row r="6">
@@ -2684,7 +2956,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45659.66819157408</v>
+        <v>45693.44248314814</v>
       </c>
     </row>
   </sheetData>
@@ -2742,7 +3014,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.6683221412</v>
+        <v>45693.44261690972</v>
       </c>
     </row>
     <row r="3">
@@ -2759,7 +3031,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.6683221412</v>
+        <v>45693.44261690972</v>
       </c>
     </row>
     <row r="4">
@@ -2776,7 +3048,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.6683221412</v>
+        <v>45693.44261690972</v>
       </c>
     </row>
     <row r="5">
@@ -2793,7 +3065,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.6683221412</v>
+        <v>45693.44261690972</v>
       </c>
     </row>
     <row r="6">
@@ -2810,7 +3082,7 @@
         <v>-0.0005</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45659.6683221412</v>
+        <v>45693.44261690972</v>
       </c>
     </row>
   </sheetData>
@@ -2868,7 +3140,7 @@
         <v>-0.0003</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66842271991</v>
+        <v>45693.4427265162</v>
       </c>
     </row>
     <row r="3">
@@ -2885,7 +3157,7 @@
         <v>-0.0003</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66842271991</v>
+        <v>45693.4427265162</v>
       </c>
     </row>
     <row r="4">
@@ -2902,7 +3174,7 @@
         <v>-0.0003</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66842271991</v>
+        <v>45693.4427265162</v>
       </c>
     </row>
   </sheetData>
@@ -2916,7 +3188,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2954,13 +3226,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.922848456476216e-30</v>
+        <v>-6.656013887802287e-30</v>
       </c>
       <c r="D2" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45659.66861936342</v>
+        <v>45693.44292105324</v>
       </c>
     </row>
     <row r="3">
@@ -2968,16 +3240,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>42655</v>
+        <v>41367</v>
       </c>
       <c r="C3" t="n">
-        <v>-8.874685183736383e-29</v>
+        <v>-1.97215226305253e-31</v>
       </c>
       <c r="D3" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45659.66861936342</v>
+        <v>45693.44292105324</v>
       </c>
     </row>
     <row r="4">
@@ -2985,16 +3257,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>43407.5</v>
+        <v>42655</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0037625</v>
+        <v>-8.993014319519535e-29</v>
       </c>
       <c r="D4" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45659.66861947917</v>
+        <v>45693.44292105324</v>
       </c>
     </row>
     <row r="5">
@@ -3002,16 +3274,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>43771.5</v>
+        <v>43407.5</v>
       </c>
       <c r="C5" t="n">
-        <v>-3.3526588471893e-30</v>
+        <v>-0.0037625</v>
       </c>
       <c r="D5" t="n">
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45659.66861936342</v>
+        <v>45693.44292125</v>
       </c>
     </row>
     <row r="6">
@@ -3019,16 +3291,33 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="n">
+        <v>43771.5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-2.662405555120915e-30</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>45693.44292105324</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="n">
         <v>44541.5</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C7" t="n">
         <v>-0.00385</v>
       </c>
-      <c r="D6" t="n">
-        <v>-5e-06</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>45659.66861947917</v>
+      <c r="D7" t="n">
+        <v>-5e-06</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>45693.44292125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update putfilter3.py to include temperature correction notes and implement viscosity; modify CSV and Excel files for consistency
</commit_message>
<xml_diff>
--- a/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
+++ b/productiecapaciteit/results/Filterweerstand/Filterweerstand_modelcoefficienten.xlsx
@@ -521,7 +521,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.44442742501</v>
+        <v>45693.44442743056</v>
       </c>
     </row>
     <row r="3">
@@ -538,7 +538,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.44442742501</v>
+        <v>45693.44442743056</v>
       </c>
     </row>
     <row r="4">
@@ -555,7 +555,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.44442742501</v>
+        <v>45693.44442743056</v>
       </c>
     </row>
     <row r="5">
@@ -572,7 +572,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45693.44442742501</v>
+        <v>45693.44442743056</v>
       </c>
     </row>
     <row r="6">
@@ -589,7 +589,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45693.44442742501</v>
+        <v>45693.44442743056</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1696,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.44398280093</v>
+        <v>45699.61820989798</v>
       </c>
     </row>
     <row r="3">
@@ -1713,7 +1713,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.44398287037</v>
+        <v>45699.61820989798</v>
       </c>
     </row>
     <row r="4">
@@ -1730,7 +1730,7 @@
         <v>-5e-06</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.44398280093</v>
+        <v>45699.61820989798</v>
       </c>
     </row>
   </sheetData>
@@ -3096,7 +3096,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3134,13 +3134,13 @@
         <v>41030</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.678513233955944e-114</v>
+        <v>-3.011893641386587e-114</v>
       </c>
       <c r="D2" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45693.4427265162</v>
+        <v>45699.44560905093</v>
       </c>
     </row>
     <row r="3">
@@ -3148,16 +3148,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>44237</v>
+        <v>43089</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.115114525930587</v>
+        <v>-0.002418679012150875</v>
       </c>
       <c r="D3" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45693.4427265162</v>
+        <v>45699.44560905093</v>
       </c>
     </row>
     <row r="4">
@@ -3165,16 +3165,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>45203</v>
+        <v>44237</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1442103368313238</v>
+        <v>-0.1151145706160745</v>
       </c>
       <c r="D4" t="n">
         <v>-0.0003</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45693.4427265162</v>
+        <v>45699.44560905093</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>45203</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.1442102341436769</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.0003</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>45699.44560905093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>